<commit_message>
updating hyperparameters with test
</commit_message>
<xml_diff>
--- a/classifier_testing/classifier_testing_parameters.xlsx
+++ b/classifier_testing/classifier_testing_parameters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1165,6 +1165,606 @@
         <v>10</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5985</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>bert_classifier_5985.pth</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5985_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E16" t="n">
+        <v>846</v>
+      </c>
+      <c r="F16" t="n">
+        <v>533</v>
+      </c>
+      <c r="G16" t="n">
+        <v>394</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>bert-large-cased-whole-word-masking</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>4</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2e-05</v>
+      </c>
+      <c r="K16" t="n">
+        <v>16</v>
+      </c>
+      <c r="L16" t="n">
+        <v>512</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.952112676056338</v>
+      </c>
+      <c r="N16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5964</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>bert_classifier_5964.pth</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>5964_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E17" t="n">
+        <v>846</v>
+      </c>
+      <c r="F17" t="n">
+        <v>533</v>
+      </c>
+      <c r="G17" t="n">
+        <v>394</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>bert-base-uncased</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>6</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="K17" t="n">
+        <v>32</v>
+      </c>
+      <c r="L17" t="n">
+        <v>256</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.9323943661971831</v>
+      </c>
+      <c r="N17" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>5537</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>bert_classifier_5537.pth</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5537_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E18" t="n">
+        <v>846</v>
+      </c>
+      <c r="F18" t="n">
+        <v>533</v>
+      </c>
+      <c r="G18" t="n">
+        <v>394</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>bert-base-uncased</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>6</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="K18" t="n">
+        <v>16</v>
+      </c>
+      <c r="L18" t="n">
+        <v>512</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.5267605633802817</v>
+      </c>
+      <c r="N18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>4223</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>bert_classifier_4223.pth</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4223_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>6412</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2690</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2140</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1582</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>bert-base-cased</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>5</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="K19" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" t="n">
+        <v>256</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.436477007014809</v>
+      </c>
+      <c r="N19" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3142</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>bert_classifier_3142.pth</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3142_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>5889</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2499</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1963</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1427</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>bert-large-uncased</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>6</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="K20" t="n">
+        <v>16</v>
+      </c>
+      <c r="L20" t="n">
+        <v>256</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.4320882852292021</v>
+      </c>
+      <c r="N20" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>805</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>bert_classifier_805.pth</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>805_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>6412</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2690</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2140</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1582</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>bert-base-uncased</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="K21" t="n">
+        <v>16</v>
+      </c>
+      <c r="L21" t="n">
+        <v>512</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.9220576773187841</v>
+      </c>
+      <c r="N21" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2344</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>bert_classifier_2344.pth</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2344_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>6412</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2690</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2140</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1582</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>bert-base-cased</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>5</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="K22" t="n">
+        <v>64</v>
+      </c>
+      <c r="L22" t="n">
+        <v>256</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.436477007014809</v>
+      </c>
+      <c r="N22" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>7918</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>bert_classifier_7918.pth</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>7918_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E23" t="n">
+        <v>846</v>
+      </c>
+      <c r="F23" t="n">
+        <v>533</v>
+      </c>
+      <c r="G23" t="n">
+        <v>394</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>bert-large-cased-whole-word-masking</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="K23" t="n">
+        <v>16</v>
+      </c>
+      <c r="L23" t="n">
+        <v>512</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.5267605633802817</v>
+      </c>
+      <c r="N23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5909</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>bert_classifier_5909.pth</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>5909_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E24" t="n">
+        <v>846</v>
+      </c>
+      <c r="F24" t="n">
+        <v>533</v>
+      </c>
+      <c r="G24" t="n">
+        <v>394</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>bert-large-uncased</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>6</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="K24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L24" t="n">
+        <v>256</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.5267605633802817</v>
+      </c>
+      <c r="N24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2290</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>bert_classifier_2290.pth</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2290_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E25" t="n">
+        <v>846</v>
+      </c>
+      <c r="F25" t="n">
+        <v>533</v>
+      </c>
+      <c r="G25" t="n">
+        <v>394</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>bert-large-cased</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>4</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2e-05</v>
+      </c>
+      <c r="K25" t="n">
+        <v>16</v>
+      </c>
+      <c r="L25" t="n">
+        <v>512</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.9352112676056338</v>
+      </c>
+      <c r="N25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>8978</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>bert_classifier_8978.pth</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>8978_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E26" t="n">
+        <v>846</v>
+      </c>
+      <c r="F26" t="n">
+        <v>533</v>
+      </c>
+      <c r="G26" t="n">
+        <v>394</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>bert-large-uncased</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>4</v>
+      </c>
+      <c r="J26" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="K26" t="n">
+        <v>8</v>
+      </c>
+      <c r="L26" t="n">
+        <v>256</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.5267605633802817</v>
+      </c>
+      <c r="N26" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3238</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>bert_classifier_3238.pth</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>3238_accuracy_scores.docx</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1773</v>
+      </c>
+      <c r="E27" t="n">
+        <v>846</v>
+      </c>
+      <c r="F27" t="n">
+        <v>533</v>
+      </c>
+      <c r="G27" t="n">
+        <v>394</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>bert-base-uncased</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>5</v>
+      </c>
+      <c r="J27" t="n">
+        <v>2e-05</v>
+      </c>
+      <c r="K27" t="n">
+        <v>32</v>
+      </c>
+      <c r="L27" t="n">
+        <v>512</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.923943661971831</v>
+      </c>
+      <c r="N27" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>